<commit_message>
Create a new workflow action to support repeating step for QC steps. New test for service. Adapted template with new dropdown option.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_identity_QC_v5_2_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_identity_QC_v5_2_0.xlsx
@@ -222,7 +222,7 @@
     <t xml:space="preserve">A03</t>
   </si>
   <si>
-    <t xml:space="preserve">Repeat step - Move to next step and repeat current step</t>
+    <t xml:space="preserve">Repeat QC step - Repeat current QC step</t>
   </si>
   <si>
     <t xml:space="preserve">D01</t>
@@ -1846,7 +1846,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.21"/>
@@ -6301,7 +6301,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="1" style="20" width="10.42"/>
   </cols>
@@ -6544,7 +6544,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.33984375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.33"/>
   </cols>
@@ -7561,10 +7561,10 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.47"/>

</xml_diff>